<commit_message>
Tidied col/group names, added planting handling
</commit_message>
<xml_diff>
--- a/app/data/parameters.xlsx
+++ b/app/data/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexg\OneDrive\Desktop\Ecodata\Repos\mars_rhino\app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D1B1D7C-C847-4D7E-83EA-DE8C4EB18FCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79DC61A6-FBCE-4A97-B677-1EE4BAEEA81B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39795" yWindow="1395" windowWidth="38700" windowHeight="15285" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="simulation_control" sheetId="1" r:id="rId1"/>
@@ -24,21 +24,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="50">
   <si>
     <t>parameter</t>
   </si>
@@ -535,7 +526,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -1001,10 +992,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2F6572E-6748-484E-9808-A0B0D9890D0A}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C84" sqref="C84"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1067,24 +1058,47 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
         <v>143</v>
       </c>
     </row>

</xml_diff>